<commit_message>
Update config file with anatomical properties
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="315">
   <si>
     <t>label</t>
   </si>
@@ -903,12 +903,81 @@
   <si>
     <t>P2286</t>
   </si>
+  <si>
+    <t>venous drainage</t>
+  </si>
+  <si>
+    <t>is venous drainage of</t>
+  </si>
+  <si>
+    <t>P2289</t>
+  </si>
+  <si>
+    <t>lymphatic drainage</t>
+  </si>
+  <si>
+    <t>is lymphatic drainage of</t>
+  </si>
+  <si>
+    <t>P2288</t>
+  </si>
+  <si>
+    <t>antagonist muscle</t>
+  </si>
+  <si>
+    <t>P2329</t>
+  </si>
+  <si>
+    <t>has anatomical branch</t>
+  </si>
+  <si>
+    <t>P3262</t>
+  </si>
+  <si>
+    <t>anatomical branch of</t>
+  </si>
+  <si>
+    <t>P3261</t>
+  </si>
+  <si>
+    <t>muscle insertion</t>
+  </si>
+  <si>
+    <t>P3491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muscle origin </t>
+  </si>
+  <si>
+    <t>P3490</t>
+  </si>
+  <si>
+    <t>innervated by</t>
+  </si>
+  <si>
+    <t>P3189</t>
+  </si>
+  <si>
+    <t>innervates</t>
+  </si>
+  <si>
+    <t>P3190</t>
+  </si>
+  <si>
+    <t>segmental innervation</t>
+  </si>
+  <si>
+    <t>is segmental innervation of</t>
+  </si>
+  <si>
+    <t>P4882</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -982,6 +1051,16 @@
       <color rgb="FF000000"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF202122"/>
+      <name val="Sans-serif"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1012,7 +1091,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1083,6 +1162,12 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -31260,7 +31345,7 @@
         <v>198</v>
       </c>
       <c r="E33" s="1" t="str">
-        <f t="shared" ref="E33:E62" si="2">D33</f>
+        <f t="shared" ref="E33:E74" si="2">D33</f>
         <v>has flow facilitated by</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -32948,8 +33033,9 @@
       <c r="D63" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>287</v>
+      <c r="E63" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>is the end time of</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>80</v>
@@ -33004,8 +33090,9 @@
       <c r="D64" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>287</v>
+      <c r="E64" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>is arterial supply of</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>37</v>
@@ -33048,18 +33135,43 @@
       <c r="AD64" s="9"/>
     </row>
     <row r="65">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
-      <c r="K65" s="9"/>
-      <c r="L65" s="9"/>
+      <c r="A65" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E65" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>is venous drainage of</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K65" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="L65" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
       <c r="O65" s="9"/>
@@ -33080,17 +33192,40 @@
       <c r="AD65" s="9"/>
     </row>
     <row r="66">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
+      <c r="A66" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="E66" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>is lymphatic drainage of</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
@@ -33112,17 +33247,40 @@
       <c r="AD66" s="9"/>
     </row>
     <row r="67">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
+      <c r="A67" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K67" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
@@ -33144,17 +33302,40 @@
       <c r="AD67" s="9"/>
     </row>
     <row r="68">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
+      <c r="A68" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
@@ -33176,17 +33357,40 @@
       <c r="AD68" s="9"/>
     </row>
     <row r="69">
-      <c r="A69" s="9"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
+      <c r="A69" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K69" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
       <c r="N69" s="9"/>
@@ -33208,17 +33412,40 @@
       <c r="AD69" s="9"/>
     </row>
     <row r="70">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
+      <c r="A70" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
       <c r="N70" s="9"/>
@@ -33240,17 +33467,40 @@
       <c r="AD70" s="9"/>
     </row>
     <row r="71">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
+      <c r="A71" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
@@ -33272,17 +33522,40 @@
       <c r="AD71" s="9"/>
     </row>
     <row r="72">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
+      <c r="A72" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H72" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K72" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
       <c r="N72" s="9"/>
@@ -33304,17 +33577,40 @@
       <c r="AD72" s="9"/>
     </row>
     <row r="73">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
+      <c r="A73" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H73" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
       <c r="N73" s="9"/>
@@ -33336,17 +33632,40 @@
       <c r="AD73" s="9"/>
     </row>
     <row r="74">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
+      <c r="A74" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E74" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>is segmental innervation of</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>

</xml_diff>

<commit_message>
Start adding support for Biological Pathway
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="331">
   <si>
     <t>label</t>
   </si>
@@ -285,6 +285,21 @@
   </si>
   <si>
     <t>Q7180990</t>
+  </si>
+  <si>
+    <t>LiverTox Toxicity Category</t>
+  </si>
+  <si>
+    <t>Q112845071</t>
+  </si>
+  <si>
+    <t>fa-skull</t>
+  </si>
+  <si>
+    <t>Biological Pathway</t>
+  </si>
+  <si>
+    <t>Q4915012</t>
   </si>
   <si>
     <t>infer_inverse</t>
@@ -679,6 +694,9 @@
     <t>is country of</t>
   </si>
   <si>
+    <t>Organization &amp; Clinical Trial</t>
+  </si>
+  <si>
     <t>P17</t>
   </si>
   <si>
@@ -986,6 +1004,21 @@
   </si>
   <si>
     <t>P6099</t>
+  </si>
+  <si>
+    <t>liver toxicity likelihood</t>
+  </si>
+  <si>
+    <t>P8026</t>
+  </si>
+  <si>
+    <t>pathway has member</t>
+  </si>
+  <si>
+    <t>member of pathway</t>
+  </si>
+  <si>
+    <t>P527</t>
   </si>
 </sst>
 </file>
@@ -2404,11 +2437,21 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="A31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2432,11 +2475,21 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -29598,34 +29651,34 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -29648,13 +29701,13 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
@@ -29670,19 +29723,19 @@
         <v>86</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
@@ -29705,13 +29758,13 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>8</v>
@@ -29727,19 +29780,19 @@
         <v>86</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="J3" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
@@ -29762,13 +29815,13 @@
     </row>
     <row r="4">
       <c r="A4" s="11" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -29784,19 +29837,19 @@
         <v>37</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
@@ -29819,19 +29872,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
@@ -29840,19 +29893,19 @@
         <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
@@ -29875,16 +29928,16 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" ref="E6:E30" si="1">D6</f>
@@ -29897,19 +29950,19 @@
         <v>37</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -29932,16 +29985,16 @@
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="1"/>
@@ -29954,19 +30007,19 @@
         <v>26</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -29989,16 +30042,16 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30011,19 +30064,19 @@
         <v>49</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -30046,16 +30099,16 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30068,19 +30121,19 @@
         <v>5</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -30103,16 +30156,16 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30125,19 +30178,19 @@
         <v>29</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -30160,16 +30213,16 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30182,19 +30235,19 @@
         <v>46</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -30217,16 +30270,16 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30239,19 +30292,19 @@
         <v>49</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -30274,13 +30327,13 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -30296,19 +30349,19 @@
         <v>49</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -30331,13 +30384,13 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -30353,19 +30406,19 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
@@ -30388,16 +30441,16 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30410,19 +30463,19 @@
         <v>17</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -30445,16 +30498,16 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30467,19 +30520,19 @@
         <v>37</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -30502,16 +30555,16 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30524,19 +30577,19 @@
         <v>9</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -30559,16 +30612,16 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30581,19 +30634,19 @@
         <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
@@ -30616,16 +30669,16 @@
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30638,19 +30691,19 @@
         <v>40</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
@@ -30673,16 +30726,16 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30695,19 +30748,19 @@
         <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
@@ -30730,41 +30783,41 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>is treated by</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
@@ -30787,16 +30840,16 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30809,19 +30862,19 @@
         <v>52</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
@@ -30844,16 +30897,16 @@
     </row>
     <row r="23">
       <c r="A23" s="11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E23" s="1" t="str">
         <f t="shared" si="1"/>
@@ -30866,19 +30919,19 @@
         <v>34</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -30901,41 +30954,41 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>may be prevented by</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
@@ -30958,41 +31011,41 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>is way of administration of</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -31015,13 +31068,13 @@
     </row>
     <row r="26">
       <c r="A26" s="11" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
@@ -31037,19 +31090,19 @@
         <v>5</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
@@ -31072,16 +31125,16 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="1"/>
@@ -31094,19 +31147,19 @@
         <v>20</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
@@ -31129,13 +31182,13 @@
     </row>
     <row r="28">
       <c r="A28" s="11" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
@@ -31151,19 +31204,19 @@
         <v>26</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
@@ -31186,16 +31239,16 @@
     </row>
     <row r="29">
       <c r="A29" s="22" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="1"/>
@@ -31208,19 +31261,19 @@
         <v>17</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
@@ -31243,13 +31296,13 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
@@ -31265,36 +31318,36 @@
         <v>9</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>49</v>
@@ -31303,36 +31356,36 @@
         <v>49</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>49</v>
@@ -31341,33 +31394,33 @@
         <v>26</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K32" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" ref="E33:E74" si="2">D33</f>
@@ -31380,19 +31433,19 @@
         <v>34</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -31415,16 +31468,16 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E34" s="1" t="str">
         <f t="shared" si="2"/>
@@ -31437,19 +31490,19 @@
         <v>32</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
@@ -31472,16 +31525,16 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E35" s="1" t="str">
         <f t="shared" si="2"/>
@@ -31494,19 +31547,19 @@
         <v>29</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
@@ -31529,13 +31582,13 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
@@ -31551,19 +31604,19 @@
         <v>17</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
@@ -31586,16 +31639,16 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E37" s="1" t="str">
         <f t="shared" si="2"/>
@@ -31608,19 +31661,19 @@
         <v>57</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
@@ -31642,41 +31695,41 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="2"/>
         <v>is country of</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>60</v>
+        <v>222</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>66</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
@@ -31698,16 +31751,16 @@
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="2"/>
@@ -31720,19 +31773,19 @@
         <v>57</v>
       </c>
       <c r="H39" s="23" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
@@ -31754,16 +31807,16 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="2"/>
@@ -31776,19 +31829,19 @@
         <v>57</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K40" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
@@ -31810,13 +31863,13 @@
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
@@ -31832,19 +31885,19 @@
         <v>60</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K41" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
@@ -31866,13 +31919,13 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
@@ -31888,19 +31941,19 @@
         <v>60</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K42" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
@@ -31922,16 +31975,16 @@
     </row>
     <row r="43">
       <c r="A43" s="22" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E43" s="1" t="str">
         <f t="shared" si="2"/>
@@ -31944,19 +31997,19 @@
         <v>60</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K43" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
@@ -31978,16 +32031,16 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32000,19 +32053,19 @@
         <v>60</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K44" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
@@ -32034,16 +32087,16 @@
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32056,19 +32109,19 @@
         <v>57</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K45" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
@@ -32090,16 +32143,16 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32112,19 +32165,19 @@
         <v>66</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K46" s="14" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
@@ -32146,16 +32199,16 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32168,19 +32221,19 @@
         <v>57</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
@@ -32202,13 +32255,13 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>8</v>
@@ -32224,19 +32277,19 @@
         <v>57</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
@@ -32258,13 +32311,13 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
@@ -32280,19 +32333,19 @@
         <v>57</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K49" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L49" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
@@ -32314,16 +32367,16 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E50" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32336,19 +32389,19 @@
         <v>57</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K50" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
@@ -32370,16 +32423,16 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E51" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32392,19 +32445,19 @@
         <v>69</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N51" s="9"/>
       <c r="O51" s="9"/>
@@ -32426,16 +32479,16 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E52" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32448,19 +32501,19 @@
         <v>57</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K52" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
@@ -32482,16 +32535,16 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E53" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32504,19 +32557,19 @@
         <v>57</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K53" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L53" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
@@ -32538,16 +32591,16 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32560,19 +32613,19 @@
         <v>63</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L54" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
@@ -32594,16 +32647,16 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32616,19 +32669,19 @@
         <v>71</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K55" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L55" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
@@ -32650,16 +32703,16 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32672,19 +32725,19 @@
         <v>57</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L56" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
@@ -32706,16 +32759,16 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32728,19 +32781,19 @@
         <v>74</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K57" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L57" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
@@ -32762,16 +32815,16 @@
     </row>
     <row r="58">
       <c r="A58" s="8" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="E58" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32784,19 +32837,19 @@
         <v>77</v>
       </c>
       <c r="H58" s="24" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K58" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L58" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
@@ -32819,16 +32872,16 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="E59" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32841,19 +32894,19 @@
         <v>9</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
@@ -32876,16 +32929,16 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="E60" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32895,22 +32948,22 @@
         <v>80</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K60" s="14" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="L60" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="M60" s="9"/>
       <c r="N60" s="9"/>
@@ -32933,16 +32986,16 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="E61" s="1" t="str">
         <f t="shared" si="2"/>
@@ -32955,19 +33008,19 @@
         <v>37</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K61" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L61" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
@@ -32990,16 +33043,16 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E62" s="1" t="str">
         <f t="shared" si="2"/>
@@ -33012,19 +33065,19 @@
         <v>82</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="K62" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L62" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
@@ -33047,16 +33100,16 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E63" s="1" t="str">
         <f t="shared" si="2"/>
@@ -33069,19 +33122,19 @@
         <v>82</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="K63" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L63" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
@@ -33104,16 +33157,16 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="E64" s="1" t="str">
         <f t="shared" si="2"/>
@@ -33126,19 +33179,19 @@
         <v>37</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K64" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
@@ -33161,16 +33214,16 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="E65" s="1" t="str">
         <f t="shared" si="2"/>
@@ -33183,19 +33236,19 @@
         <v>37</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K65" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
@@ -33218,16 +33271,16 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E66" s="1" t="str">
         <f t="shared" si="2"/>
@@ -33240,19 +33293,19 @@
         <v>37</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K66" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
@@ -33275,13 +33328,13 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>8</v>
@@ -33297,19 +33350,19 @@
         <v>37</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K67" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L67" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
@@ -33332,13 +33385,13 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>8</v>
@@ -33354,19 +33407,19 @@
         <v>37</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K68" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L68" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
@@ -33389,13 +33442,13 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>8</v>
@@ -33411,19 +33464,19 @@
         <v>37</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K69" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M69" s="9"/>
       <c r="N69" s="9"/>
@@ -33446,13 +33499,13 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>8</v>
@@ -33468,19 +33521,19 @@
         <v>37</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K70" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M70" s="9"/>
       <c r="N70" s="9"/>
@@ -33503,13 +33556,13 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>8</v>
@@ -33525,19 +33578,19 @@
         <v>37</v>
       </c>
       <c r="H71" s="25" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K71" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
@@ -33560,13 +33613,13 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>8</v>
@@ -33582,19 +33635,19 @@
         <v>37</v>
       </c>
       <c r="H72" s="26" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K72" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M72" s="9"/>
       <c r="N72" s="9"/>
@@ -33617,13 +33670,13 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>8</v>
@@ -33639,19 +33692,19 @@
         <v>37</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K73" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L73" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M73" s="9"/>
       <c r="N73" s="9"/>
@@ -33674,16 +33727,16 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="E74" s="1" t="str">
         <f t="shared" si="2"/>
@@ -33696,19 +33749,19 @@
         <v>37</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K74" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L74" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>
@@ -33731,13 +33784,13 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>8</v>
@@ -33752,19 +33805,19 @@
         <v>89</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J75" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K75" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
@@ -33786,18 +33839,42 @@
       <c r="AD75" s="9"/>
     </row>
     <row r="76">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
+      <c r="A76" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J76" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="L76" s="7" t="s">
+        <v>219</v>
+      </c>
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
       <c r="O76" s="9"/>
@@ -33818,18 +33895,43 @@
       <c r="AD76" s="9"/>
     </row>
     <row r="77">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
+      <c r="A77" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="E77" s="9" t="str">
+        <f>D77</f>
+        <v>member of pathway</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K77" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="L77" s="7" t="s">
+        <v>219</v>
+      </c>
       <c r="M77" s="9"/>
       <c r="N77" s="9"/>
       <c r="O77" s="9"/>

</xml_diff>

<commit_message>
Update the Sparnatural config
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="359">
   <si>
     <t>label</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Disease</t>
   </si>
   <si>
-    <t>Q12136</t>
+    <t>Q112193867</t>
   </si>
   <si>
     <t>fa-viruses</t>
@@ -53,16 +53,16 @@
     <t>abnormal condition negatively affecting organisms</t>
   </si>
   <si>
-    <t>Q112193867</t>
+    <t>Symptom or Sign</t>
   </si>
   <si>
-    <t>Symptom</t>
-  </si>
-  <si>
-    <t>Q169872</t>
+    <t>Q112965645</t>
   </si>
   <si>
     <t>fa-head-side-cough</t>
+  </si>
+  <si>
+    <t>departure from normal function or feeling, reflecting the presence of an unusual state</t>
   </si>
   <si>
     <t>Gene</t>
@@ -125,10 +125,10 @@
     <t>fa-flask</t>
   </si>
   <si>
-    <t>Anatomical Structure</t>
+    <t>Anatomical Entity</t>
   </si>
   <si>
-    <t>Q4936952</t>
+    <t>Q112826905</t>
   </si>
   <si>
     <t>fa-lungs</t>
@@ -505,10 +505,10 @@
     <t>P7500</t>
   </si>
   <si>
-    <t>has symptom</t>
+    <t>has Symptom or Sign</t>
   </si>
   <si>
-    <t>symptom of</t>
+    <t>Symptom or Sign of</t>
   </si>
   <si>
     <t>P780</t>
@@ -1020,6 +1020,90 @@
   <si>
     <t>P527</t>
   </si>
+  <si>
+    <t>is found in taxon</t>
+  </si>
+  <si>
+    <t>the taxon where this entity is found</t>
+  </si>
+  <si>
+    <t>is taxon where is found</t>
+  </si>
+  <si>
+    <t>Gene &amp; Protein</t>
+  </si>
+  <si>
+    <t>P703</t>
+  </si>
+  <si>
+    <t>positive therapeutic predictor for</t>
+  </si>
+  <si>
+    <t>has positive therapeutic predictor</t>
+  </si>
+  <si>
+    <t>the presence of the genetic variant helps to predict good response to a treatment</t>
+  </si>
+  <si>
+    <t>P3354</t>
+  </si>
+  <si>
+    <t>negative therapeutic predictor for</t>
+  </si>
+  <si>
+    <t>has negative therapeutic predictor</t>
+  </si>
+  <si>
+    <t>the presence of the genetic variant helps to predict no response or resistance to a treatment</t>
+  </si>
+  <si>
+    <t>P3355</t>
+  </si>
+  <si>
+    <t>positive diagnostic predictor for</t>
+  </si>
+  <si>
+    <t>has positive prognostic predictor</t>
+  </si>
+  <si>
+    <t>the presence of the genetic variant helps to diagnose the presence of disease, used as inclusion criteria</t>
+  </si>
+  <si>
+    <t>P3356</t>
+  </si>
+  <si>
+    <t>negative diagnostic predictor for</t>
+  </si>
+  <si>
+    <t>has negative diagnostic predictor</t>
+  </si>
+  <si>
+    <t>the presence of the genetic variant helps to diagnose the absence of disease, used as exclusion criteria</t>
+  </si>
+  <si>
+    <t>P3357</t>
+  </si>
+  <si>
+    <t>positive prognostic predictor for</t>
+  </si>
+  <si>
+    <t>the prognostic of the disease is generally better when this variant is present</t>
+  </si>
+  <si>
+    <t>P3358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative prognostic predictor for </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has negative prognostic predictor </t>
+  </si>
+  <si>
+    <t>the prognostic of the disease is generally worst when this variant is present</t>
+  </si>
+  <si>
+    <t>P3359</t>
+  </si>
 </sst>
 </file>
 
@@ -1533,7 +1617,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1559,16 +1643,16 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -29634,10 +29718,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="24.88"/>
+    <col customWidth="1" min="1" max="1" width="33.25"/>
+    <col customWidth="1" min="2" max="2" width="24.88"/>
     <col customWidth="1" min="3" max="3" width="10.5"/>
     <col customWidth="1" min="4" max="4" width="11.63"/>
-    <col customWidth="1" min="5" max="6" width="20.25"/>
+    <col customWidth="1" min="5" max="5" width="18.63"/>
+    <col customWidth="1" min="6" max="6" width="20.25"/>
     <col customWidth="1" min="7" max="7" width="21.88"/>
     <col customWidth="1" min="8" max="8" width="20.5"/>
     <col customWidth="1" min="9" max="9" width="8.13"/>
@@ -29725,7 +29811,7 @@
       </c>
       <c r="G2" s="9" t="str">
         <f>JOIN(" &amp; ",classes!A2:A27)</f>
-        <v>Pharmaceutical Product &amp; Disease &amp; Symptom &amp; Gene &amp; Chromosome &amp; Cell Type &amp; Protein &amp; Biological Process &amp; Cell Component &amp; Chemical Compound &amp; Anatomical Structure &amp; Medical Test &amp; Route of Administration &amp; Mode of Inheritance &amp; Organism &amp; US Pregnancy Category &amp; Gene Variant &amp; Person &amp; Organization &amp; Publication &amp; Country &amp; Publisher &amp; Specialty &amp; Access Status &amp; Award &amp; Clinical Trial</v>
+        <v>Pharmaceutical Product &amp; Disease &amp; Symptom or Sign &amp; Gene &amp; Chromosome &amp; Cell Type &amp; Protein &amp; Biological Process &amp; Cell Component &amp; Chemical Compound &amp; Anatomical Entity &amp; Medical Test &amp; Route of Administration &amp; Mode of Inheritance &amp; Organism &amp; US Pregnancy Category &amp; Gene Variant &amp; Person &amp; Organization &amp; Publication &amp; Country &amp; Publisher &amp; Specialty &amp; Access Status &amp; Award &amp; Clinical Trial</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>86</v>
@@ -29785,7 +29871,7 @@
       </c>
       <c r="G3" s="9" t="str">
         <f>JOIN(" &amp; ",classes!A3:A28)</f>
-        <v>Disease &amp; Symptom &amp; Gene &amp; Chromosome &amp; Cell Type &amp; Protein &amp; Biological Process &amp; Cell Component &amp; Chemical Compound &amp; Anatomical Structure &amp; Medical Test &amp; Route of Administration &amp; Mode of Inheritance &amp; Organism &amp; US Pregnancy Category &amp; Gene Variant &amp; Person &amp; Organization &amp; Publication &amp; Country &amp; Publisher &amp; Specialty &amp; Access Status &amp; Award &amp; Clinical Trial &amp; Date</v>
+        <v>Disease &amp; Symptom or Sign &amp; Gene &amp; Chromosome &amp; Cell Type &amp; Protein &amp; Biological Process &amp; Cell Component &amp; Chemical Compound &amp; Anatomical Entity &amp; Medical Test &amp; Route of Administration &amp; Mode of Inheritance &amp; Organism &amp; US Pregnancy Category &amp; Gene Variant &amp; Person &amp; Organization &amp; Publication &amp; Country &amp; Publisher &amp; Specialty &amp; Access Status &amp; Award &amp; Clinical Trial &amp; Date</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>86</v>
@@ -30681,13 +30767,13 @@
       </c>
       <c r="F18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>symptom of</v>
+        <v>Symptom or Sign of</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>161</v>
@@ -30807,7 +30893,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>167</v>
@@ -34162,7 +34248,7 @@
         <v>119</v>
       </c>
       <c r="M77" s="7" t="s">
-        <v>219</v>
+        <v>120</v>
       </c>
       <c r="N77" s="9"/>
       <c r="O77" s="9"/>
@@ -34184,19 +34270,45 @@
       <c r="AE77" s="9"/>
     </row>
     <row r="78">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
-      <c r="M78" s="9"/>
+      <c r="A78" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K78" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L78" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M78" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="N78" s="9"/>
       <c r="O78" s="9"/>
       <c r="P78" s="9"/>
@@ -34217,19 +34329,45 @@
       <c r="AE78" s="9"/>
     </row>
     <row r="79">
-      <c r="A79" s="9"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
-      <c r="K79" s="9"/>
-      <c r="L79" s="9"/>
-      <c r="M79" s="9"/>
+      <c r="A79" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="J79" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K79" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L79" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M79" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="N79" s="9"/>
       <c r="O79" s="9"/>
       <c r="P79" s="9"/>
@@ -34250,19 +34388,45 @@
       <c r="AE79" s="9"/>
     </row>
     <row r="80">
-      <c r="A80" s="9"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="9"/>
-      <c r="J80" s="9"/>
-      <c r="K80" s="9"/>
-      <c r="L80" s="9"/>
-      <c r="M80" s="9"/>
+      <c r="A80" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="G80" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="J80" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K80" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L80" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M80" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="N80" s="9"/>
       <c r="O80" s="9"/>
       <c r="P80" s="9"/>
@@ -34283,19 +34447,45 @@
       <c r="AE80" s="9"/>
     </row>
     <row r="81">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="9"/>
-      <c r="L81" s="9"/>
-      <c r="M81" s="9"/>
+      <c r="A81" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="J81" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K81" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M81" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="N81" s="9"/>
       <c r="O81" s="9"/>
       <c r="P81" s="9"/>
@@ -34316,19 +34506,45 @@
       <c r="AE81" s="9"/>
     </row>
     <row r="82">
-      <c r="A82" s="9"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
-      <c r="J82" s="9"/>
-      <c r="K82" s="9"/>
-      <c r="L82" s="9"/>
-      <c r="M82" s="9"/>
+      <c r="A82" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K82" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L82" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M82" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="N82" s="9"/>
       <c r="O82" s="9"/>
       <c r="P82" s="9"/>
@@ -34349,19 +34565,45 @@
       <c r="AE82" s="9"/>
     </row>
     <row r="83">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
-      <c r="I83" s="9"/>
-      <c r="J83" s="9"/>
-      <c r="K83" s="9"/>
-      <c r="L83" s="9"/>
-      <c r="M83" s="9"/>
+      <c r="A83" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="J83" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K83" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L83" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M83" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="N83" s="9"/>
       <c r="O83" s="9"/>
       <c r="P83" s="9"/>
@@ -34382,19 +34624,45 @@
       <c r="AE83" s="9"/>
     </row>
     <row r="84">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
-      <c r="J84" s="9"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="9"/>
+      <c r="A84" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J84" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K84" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M84" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="N84" s="9"/>
       <c r="O84" s="9"/>
       <c r="P84" s="9"/>
@@ -34415,7 +34683,7 @@
       <c r="AE84" s="9"/>
     </row>
     <row r="85">
-      <c r="A85" s="9"/>
+      <c r="A85" s="7"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
@@ -34448,7 +34716,7 @@
       <c r="AE85" s="9"/>
     </row>
     <row r="86">
-      <c r="A86" s="9"/>
+      <c r="A86" s="7"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
@@ -34481,7 +34749,7 @@
       <c r="AE86" s="9"/>
     </row>
     <row r="87">
-      <c r="A87" s="9"/>
+      <c r="A87" s="7"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
@@ -34514,7 +34782,6 @@
       <c r="AE87" s="9"/>
     </row>
     <row r="88">
-      <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>

</xml_diff>